<commit_message>
Updated crash stats and R script
</commit_message>
<xml_diff>
--- a/historical crashes.xlsx
+++ b/historical crashes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -78,6 +78,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -125,7 +128,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -160,7 +163,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -369,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +487,7 @@
         <v>1936</v>
       </c>
       <c r="B7">
-        <v>755</v>
+        <v>755765</v>
       </c>
       <c r="C7">
         <v>11388</v>
@@ -953,6 +956,805 @@
       </c>
       <c r="E34">
         <v>47801</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1964</v>
+      </c>
+      <c r="B35">
+        <v>2694023</v>
+      </c>
+      <c r="C35">
+        <v>111232</v>
+      </c>
+      <c r="D35">
+        <v>1424</v>
+      </c>
+      <c r="E35">
+        <v>54560</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1965</v>
+      </c>
+      <c r="B36">
+        <v>2739138</v>
+      </c>
+      <c r="C36">
+        <v>128462</v>
+      </c>
+      <c r="D36">
+        <v>1611</v>
+      </c>
+      <c r="E36">
+        <v>60917</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1966</v>
+      </c>
+      <c r="B37">
+        <v>2821648</v>
+      </c>
+      <c r="C37">
+        <v>139781</v>
+      </c>
+      <c r="D37">
+        <v>1596</v>
+      </c>
+      <c r="E37">
+        <v>65210</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1967</v>
+      </c>
+      <c r="B38">
+        <v>3004654</v>
+      </c>
+      <c r="C38">
+        <v>145008</v>
+      </c>
+      <c r="D38">
+        <v>1719</v>
+      </c>
+      <c r="E38">
+        <v>67280</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1968</v>
+      </c>
+      <c r="B39">
+        <v>3128509</v>
+      </c>
+      <c r="C39">
+        <v>155127</v>
+      </c>
+      <c r="D39">
+        <v>1586</v>
+      </c>
+      <c r="E39">
+        <v>71520</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1969</v>
+      </c>
+      <c r="B40">
+        <v>3247979</v>
+      </c>
+      <c r="C40">
+        <v>169395</v>
+      </c>
+      <c r="D40">
+        <v>1683</v>
+      </c>
+      <c r="E40">
+        <v>74902</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1970</v>
+      </c>
+      <c r="B41">
+        <v>3422892</v>
+      </c>
+      <c r="C41">
+        <v>141609</v>
+      </c>
+      <c r="D41">
+        <v>1535</v>
+      </c>
+      <c r="E41">
+        <v>75126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1971</v>
+      </c>
+      <c r="B42">
+        <v>3563197</v>
+      </c>
+      <c r="C42">
+        <v>158831</v>
+      </c>
+      <c r="D42">
+        <v>1769</v>
+      </c>
+      <c r="E42">
+        <v>84650</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1972</v>
+      </c>
+      <c r="B43">
+        <v>3688541</v>
+      </c>
+      <c r="C43">
+        <v>189494</v>
+      </c>
+      <c r="D43">
+        <v>1934</v>
+      </c>
+      <c r="E43">
+        <v>95181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1973</v>
+      </c>
+      <c r="B44">
+        <v>3841628</v>
+      </c>
+      <c r="C44">
+        <v>193021</v>
+      </c>
+      <c r="D44">
+        <v>1959</v>
+      </c>
+      <c r="E44">
+        <v>97790</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1974</v>
+      </c>
+      <c r="B45">
+        <v>3972980</v>
+      </c>
+      <c r="C45">
+        <v>204271</v>
+      </c>
+      <c r="D45">
+        <v>1748</v>
+      </c>
+      <c r="E45">
+        <v>98673</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1975</v>
+      </c>
+      <c r="B46">
+        <v>4160623</v>
+      </c>
+      <c r="C46">
+        <v>213689</v>
+      </c>
+      <c r="D46">
+        <v>1800</v>
+      </c>
+      <c r="E46">
+        <v>97034</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1976</v>
+      </c>
+      <c r="B47">
+        <v>4315925</v>
+      </c>
+      <c r="C47">
+        <v>211865</v>
+      </c>
+      <c r="D47">
+        <v>1511</v>
+      </c>
+      <c r="E47">
+        <v>83736</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1977</v>
+      </c>
+      <c r="B48">
+        <v>4562903</v>
+      </c>
+      <c r="C48">
+        <v>218567</v>
+      </c>
+      <c r="D48">
+        <v>1420</v>
+      </c>
+      <c r="E48">
+        <v>95964</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1978</v>
+      </c>
+      <c r="B49">
+        <v>4725546</v>
+      </c>
+      <c r="C49">
+        <v>186363</v>
+      </c>
+      <c r="D49">
+        <v>1450</v>
+      </c>
+      <c r="E49">
+        <v>94979</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1979</v>
+      </c>
+      <c r="B50">
+        <v>4858351</v>
+      </c>
+      <c r="C50">
+        <v>197196</v>
+      </c>
+      <c r="D50">
+        <v>1560</v>
+      </c>
+      <c r="E50">
+        <v>101321</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1980</v>
+      </c>
+      <c r="B51">
+        <v>4993531</v>
+      </c>
+      <c r="C51">
+        <v>196501</v>
+      </c>
+      <c r="D51">
+        <v>1508</v>
+      </c>
+      <c r="E51">
+        <v>101367</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1981</v>
+      </c>
+      <c r="B52">
+        <v>5123177</v>
+      </c>
+      <c r="C52">
+        <v>198372</v>
+      </c>
+      <c r="D52">
+        <v>1445</v>
+      </c>
+      <c r="E52">
+        <v>100321</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1982</v>
+      </c>
+      <c r="B53">
+        <v>5247198</v>
+      </c>
+      <c r="C53">
+        <v>187943</v>
+      </c>
+      <c r="D53">
+        <v>1138</v>
+      </c>
+      <c r="E53">
+        <v>92815</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1983</v>
+      </c>
+      <c r="B54">
+        <v>5380259</v>
+      </c>
+      <c r="C54">
+        <v>181999</v>
+      </c>
+      <c r="D54">
+        <v>1204</v>
+      </c>
+      <c r="E54">
+        <v>91706</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1984</v>
+      </c>
+      <c r="B55">
+        <v>5513911</v>
+      </c>
+      <c r="C55">
+        <v>194782</v>
+      </c>
+      <c r="D55">
+        <v>1132</v>
+      </c>
+      <c r="E55">
+        <v>97230</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1985</v>
+      </c>
+      <c r="B56">
+        <v>5660422</v>
+      </c>
+      <c r="C56">
+        <v>189750</v>
+      </c>
+      <c r="D56">
+        <v>1191</v>
+      </c>
+      <c r="E56">
+        <v>109169</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1986</v>
+      </c>
+      <c r="B57">
+        <v>5817799</v>
+      </c>
+      <c r="C57">
+        <v>187286</v>
+      </c>
+      <c r="D57">
+        <v>1102</v>
+      </c>
+      <c r="E57">
+        <v>108839</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1987</v>
+      </c>
+      <c r="B58">
+        <v>5978105</v>
+      </c>
+      <c r="C58">
+        <v>203431</v>
+      </c>
+      <c r="D58">
+        <v>1229</v>
+      </c>
+      <c r="E58">
+        <v>121089</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1988</v>
+      </c>
+      <c r="B59">
+        <v>6118112</v>
+      </c>
+      <c r="C59">
+        <v>228398</v>
+      </c>
+      <c r="D59">
+        <v>1237</v>
+      </c>
+      <c r="E59">
+        <v>118158</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1989</v>
+      </c>
+      <c r="B60">
+        <v>6290424</v>
+      </c>
+      <c r="C60">
+        <v>247038</v>
+      </c>
+      <c r="D60">
+        <v>1286</v>
+      </c>
+      <c r="E60">
+        <v>120652</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1990</v>
+      </c>
+      <c r="B61">
+        <v>6448883</v>
+      </c>
+      <c r="C61">
+        <v>220188</v>
+      </c>
+      <c r="D61">
+        <v>1120</v>
+      </c>
+      <c r="E61">
+        <v>101575</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1991</v>
+      </c>
+      <c r="B62">
+        <v>6574231</v>
+      </c>
+      <c r="C62">
+        <v>213669</v>
+      </c>
+      <c r="D62">
+        <v>1102</v>
+      </c>
+      <c r="E62">
+        <v>90519</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1992</v>
+      </c>
+      <c r="B63">
+        <v>6688761</v>
+      </c>
+      <c r="C63">
+        <v>224249</v>
+      </c>
+      <c r="D63">
+        <v>1090</v>
+      </c>
+      <c r="E63">
+        <v>91025</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1993</v>
+      </c>
+      <c r="B64">
+        <v>6823428</v>
+      </c>
+      <c r="C64">
+        <v>228834</v>
+      </c>
+      <c r="D64">
+        <v>1135</v>
+      </c>
+      <c r="E64">
+        <v>91149</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1994</v>
+      </c>
+      <c r="B65">
+        <v>6983960</v>
+      </c>
+      <c r="C65">
+        <v>226996</v>
+      </c>
+      <c r="D65">
+        <v>999</v>
+      </c>
+      <c r="E65">
+        <v>90030</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1995</v>
+      </c>
+      <c r="B66">
+        <v>7086018</v>
+      </c>
+      <c r="C66">
+        <v>219085</v>
+      </c>
+      <c r="D66">
+        <v>999</v>
+      </c>
+      <c r="E66">
+        <v>89572</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1996</v>
+      </c>
+      <c r="B67">
+        <v>7258167</v>
+      </c>
+      <c r="C67">
+        <v>215024</v>
+      </c>
+      <c r="D67">
+        <v>929</v>
+      </c>
+      <c r="E67">
+        <v>88445</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1997</v>
+      </c>
+      <c r="B68">
+        <v>7537607</v>
+      </c>
+      <c r="C68">
+        <v>221500</v>
+      </c>
+      <c r="D68">
+        <v>899</v>
+      </c>
+      <c r="E68">
+        <v>85527</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>1998</v>
+      </c>
+      <c r="B69">
+        <v>7727756</v>
+      </c>
+      <c r="C69">
+        <v>213356</v>
+      </c>
+      <c r="D69">
+        <v>854</v>
+      </c>
+      <c r="E69">
+        <v>83154</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>1999</v>
+      </c>
+      <c r="B70">
+        <v>7918314</v>
+      </c>
+      <c r="C70">
+        <v>221962</v>
+      </c>
+      <c r="D70">
+        <v>868</v>
+      </c>
+      <c r="E70">
+        <v>84062</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>2000</v>
+      </c>
+      <c r="B71">
+        <v>8121374</v>
+      </c>
+      <c r="C71">
+        <v>240630</v>
+      </c>
+      <c r="D71">
+        <v>849</v>
+      </c>
+      <c r="E71">
+        <v>85009</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>2001</v>
+      </c>
+      <c r="B72">
+        <v>8266616</v>
+      </c>
+      <c r="C72">
+        <v>234004</v>
+      </c>
+      <c r="D72">
+        <v>845</v>
+      </c>
+      <c r="E72">
+        <v>81782</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>2002</v>
+      </c>
+      <c r="B73">
+        <v>8413504</v>
+      </c>
+      <c r="C73">
+        <v>244642</v>
+      </c>
+      <c r="D73">
+        <v>873</v>
+      </c>
+      <c r="E73">
+        <v>84192</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2003</v>
+      </c>
+      <c r="B74">
+        <v>8541555</v>
+      </c>
+      <c r="C74">
+        <v>246463</v>
+      </c>
+      <c r="D74">
+        <v>831</v>
+      </c>
+      <c r="E74">
+        <v>77879</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>2004</v>
+      </c>
+      <c r="B75">
+        <v>8655597</v>
+      </c>
+      <c r="C75">
+        <v>231548</v>
+      </c>
+      <c r="D75">
+        <v>799</v>
+      </c>
+      <c r="E75">
+        <v>73008</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>2005</v>
+      </c>
+      <c r="B76">
+        <v>8762210</v>
+      </c>
+      <c r="C76">
+        <v>230258</v>
+      </c>
+      <c r="D76">
+        <v>766</v>
+      </c>
+      <c r="E76">
+        <v>71850</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>2006</v>
+      </c>
+      <c r="B77">
+        <v>8867965</v>
+      </c>
+      <c r="C77">
+        <v>216247</v>
+      </c>
+      <c r="D77">
+        <v>769</v>
+      </c>
+      <c r="E77">
+        <v>68793</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>2007</v>
+      </c>
+      <c r="B78">
+        <v>8945397</v>
+      </c>
+      <c r="C78">
+        <v>233487</v>
+      </c>
+      <c r="D78">
+        <v>765</v>
+      </c>
+      <c r="E78">
+        <v>67175</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>2008</v>
+      </c>
+      <c r="B79">
+        <v>9042286</v>
+      </c>
+      <c r="C79">
+        <v>229196</v>
+      </c>
+      <c r="D79">
+        <v>631</v>
+      </c>
+      <c r="E79">
+        <v>62743</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>2009</v>
+      </c>
+      <c r="B80">
+        <v>9101938</v>
+      </c>
+      <c r="C80">
+        <v>216315</v>
+      </c>
+      <c r="D80">
+        <v>564</v>
+      </c>
+      <c r="E80">
+        <v>62562</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>2010</v>
+      </c>
+      <c r="B81">
+        <v>9245267</v>
+      </c>
+      <c r="C81">
+        <v>215533</v>
+      </c>
+      <c r="D81">
+        <v>579</v>
+      </c>
+      <c r="E81">
+        <v>64514</v>
       </c>
     </row>
   </sheetData>

</xml_diff>